<commit_message>
Updated files and bill of material in B645
</commit_message>
<xml_diff>
--- a/System_development/magnet_design/B645_Tesla_magnet/B645_BillofMaterials.xlsx
+++ b/System_development/magnet_design/B645_Tesla_magnet/B645_BillofMaterials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adowney2\Documents\GitHub\Compact-NMR\System_development\magnet_design\B645_Tesla_magnet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\OneDrive - Georgia Southern University\Desktop\USC-1stSemester\NMR\Compact-NMR\System_development\magnet_design\B645_Tesla_magnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D0588-CCBC-472F-ABB2-D6264B7206FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAC95E1-8886-4616-A141-8F4A5CC9C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillofMaterials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>https://www.grainger.com/product/Carbon-Steel-Rectangular-Bar-782V02</t>
+  </si>
+  <si>
+    <t>0.75 in Thick, 3 1/2 in x 12 in</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/Carbon-Steel-Rectangular-Bar-2HHR7</t>
   </si>
 </sst>
 </file>
@@ -947,24 +953,24 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.796875" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" customWidth="1"/>
-    <col min="6" max="6" width="62.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -984,7 +990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1005,52 +1011,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>38.81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="4"/>
     </row>
   </sheetData>

</xml_diff>